<commit_message>
Adding updated files remove pclody conflict
</commit_message>
<xml_diff>
--- a/Testinput/Inputsheet.xlsx
+++ b/Testinput/Inputsheet.xlsx
@@ -8,27 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation-Workspace\Ymca\Testinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4F9DA6-6D85-4DF1-822F-536280C443DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0069B512-9105-48A2-9E78-3DCBCE99E10E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mastertestcases" sheetId="1" r:id="rId1"/>
-    <sheet name="CloudAndroid" sheetId="30" r:id="rId2"/>
-    <sheet name="CloudiOS" sheetId="31" r:id="rId3"/>
-    <sheet name="IOS" sheetId="26" r:id="rId4"/>
-    <sheet name="Google" sheetId="20" r:id="rId5"/>
-    <sheet name="Google2" sheetId="25" r:id="rId6"/>
-    <sheet name="Google3" sheetId="27" r:id="rId7"/>
-    <sheet name="API" sheetId="28" r:id="rId8"/>
-    <sheet name="MethodsDropDown" sheetId="29" r:id="rId9"/>
+    <sheet name="AndroidTest" sheetId="32" r:id="rId2"/>
+    <sheet name="IOSTest" sheetId="26" r:id="rId3"/>
+    <sheet name="LocalBrowser" sheetId="20" r:id="rId4"/>
+    <sheet name="BrowserStackTest" sheetId="33" r:id="rId5"/>
+    <sheet name="SauceLabsTest" sheetId="27" r:id="rId6"/>
+    <sheet name="API" sheetId="28" r:id="rId7"/>
+    <sheet name="CloudAndroid" sheetId="30" r:id="rId8"/>
+    <sheet name="CloudiOS" sheetId="31" r:id="rId9"/>
+    <sheet name="MethodsDropDown" sheetId="29" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="168">
   <si>
     <t>TCID</t>
   </si>
@@ -81,9 +82,6 @@
     <t>closeapplication</t>
   </si>
   <si>
-    <t>Google</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -126,9 +124,6 @@
     <t>TC003</t>
   </si>
   <si>
-    <t>IOS</t>
-  </si>
-  <si>
     <t>launchapplication</t>
   </si>
   <si>
@@ -153,9 +148,6 @@
     <t>Googlee</t>
   </si>
   <si>
-    <t>Google2</t>
-  </si>
-  <si>
     <t>Enter Text</t>
   </si>
   <si>
@@ -169,9 +161,6 @@
   </si>
   <si>
     <t>FirstOption</t>
-  </si>
-  <si>
-    <t>Google3</t>
   </si>
   <si>
     <t>TC004</t>
@@ -507,6 +496,45 @@
   </si>
   <si>
     <t>AndoidNextButton</t>
+  </si>
+  <si>
+    <t>android</t>
+  </si>
+  <si>
+    <t>ios</t>
+  </si>
+  <si>
+    <t>browserstack</t>
+  </si>
+  <si>
+    <t>browserstackchrome</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>saucelabs</t>
+  </si>
+  <si>
+    <t>saucelabschrome</t>
+  </si>
+  <si>
+    <t>AndroidTest</t>
+  </si>
+  <si>
+    <t>IOSTest</t>
+  </si>
+  <si>
+    <t>LocalBrowser</t>
+  </si>
+  <si>
+    <t>BrowserStackTest</t>
+  </si>
+  <si>
+    <t>SauceLabsTest</t>
+  </si>
+  <si>
+    <t>cloudAndroid</t>
   </si>
 </sst>
 </file>
@@ -1071,16 +1099,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.453125" style="5" customWidth="1"/>
     <col min="5" max="16384" width="9" style="5"/>
@@ -1105,10 +1133,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -1117,7 +1145,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>165</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
@@ -1126,22 +1154,22 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>163</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -1150,44 +1178,56 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C8" xr:uid="{5E446159-0A27-42AD-94DD-5B5984818C09}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{5E446159-0A27-42AD-94DD-5B5984818C09}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1196,425 +1236,471 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DC243D4-1802-4B2F-A8E1-29C13F5D35F7}">
-  <dimension ref="A1:K5"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B7F41E-692A-4CA8-9ED3-CAEF988BE607}">
+  <dimension ref="A1:A88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.90625" style="5"/>
+    <col min="1" max="1" width="28.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="7" t="s">
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="3"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4" xr:uid="{31172039-31F4-40D8-A07C-07B2088B0032}">
-      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{B84BEFCF-B23D-47BD-9339-A47E1F0E0935}">
-      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{D8B78352-178C-4E82-B43C-257CA3FB785E}">
-      <formula1>"ios,android,cloudAndroid,CloudiOS,NA"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF15D293-9E7B-4DB5-A90A-7077A9C8C42F}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD96CCB-A1A6-4ED0-8D30-67999F5EF9B1}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="15.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.5">
-      <c r="A3" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.5">
-      <c r="A4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2">
-        <v>801742</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.5">
-      <c r="A5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="3"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{C74B8B57-87F6-4358-A16B-E2E274F68C56}">
-      <formula1>"ios,android,cloudAndroid,CloudiOS,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{CB583239-9D7D-4A1B-AE71-C48E4BC43385}">
-      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4" xr:uid="{345E68F6-2630-4998-85A7-A066C14B1EB0}">
-      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB22AF6-DB92-475E-8397-BFEB0405B8C4}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1638,31 +1724,238 @@
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{46257E2C-578E-4299-893D-8DC7B6E23189}">
+      <formula1>"ios,android,cloudAndroid,CloudiOS,NA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{23951901-8F95-4C28-B671-572E3C0FB9DA}">
+      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4" xr:uid="{66E58A67-28A0-48BD-B382-68BF4E4214FB}">
+      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB22AF6-DB92-475E-8397-BFEB0405B8C4}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.90625" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
@@ -1670,7 +1963,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>10</v>
@@ -1691,10 +1984,10 @@
         <v>11</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>11</v>
@@ -1703,13 +1996,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>14</v>
@@ -1736,13 +2029,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>14</v>
@@ -1769,13 +2062,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
@@ -1825,12 +2118,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E63851-4616-491C-89B9-1AFD437E032E}">
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1853,31 +2146,31 @@
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
@@ -1903,7 +2196,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>11</v>
@@ -1918,7 +2211,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -1930,7 +2223,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>11</v>
@@ -1951,10 +2244,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
@@ -1963,7 +2256,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>11</v>
@@ -1984,19 +2277,19 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>11</v>
@@ -2017,13 +2310,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>14</v>
@@ -2050,7 +2343,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>16</v>
@@ -2117,27 +2410,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BA64C3-74D1-4FB7-85C0-F4FDCDDA50C6}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFA2299-BAF5-4AEB-8201-9BE12BC72674}">
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.54296875" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="5"/>
+    <col min="11" max="11" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2145,31 +2438,31 @@
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
@@ -2195,10 +2488,10 @@
         <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>30</v>
+        <v>158</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>11</v>
+        <v>157</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>11</v>
@@ -2210,7 +2503,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -2222,7 +2515,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>11</v>
@@ -2243,10 +2536,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
@@ -2255,7 +2548,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>11</v>
@@ -2276,19 +2569,19 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>11</v>
@@ -2309,13 +2602,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>14</v>
@@ -2342,7 +2635,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>16</v>
@@ -2375,28 +2668,29 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{4F9D7357-4028-4F42-8424-AE9342FEA69C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{25F55D36-9777-4009-A415-EC6180727EA8}">
       <formula1>"ios,android,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{929A75F1-AF4D-4DB8-A6A6-BD8C8E4B4C4F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{BB2605B6-0E53-4E54-BE61-FD1BB39326EF}">
       <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{A4595E7C-BD04-461D-8437-84C02516D103}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{307608A3-E9A9-4B8B-BBE5-81D2DE6262A1}">
       <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D2:D4" xr:uid="{2B7611BD-935C-4658-88F0-967E807170F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D2:D4" xr:uid="{F9AF23F6-16A3-4F2C-8DDE-2BD1876D8B36}">
       <formula1>"NA,xpath,id,name,linktext,partiallinktext"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://accounts.google.com/" xr:uid="{ADBAAD69-22FB-4324-A727-290B4AC4217D}"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://accounts.google.com/" xr:uid="{B4460FB1-2BEB-422D-933E-0552D390B5D8}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://accounts.google.com/" xr:uid="{95230630-795B-4083-82BB-802F375C76C1}"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://accounts.google.com/" xr:uid="{523DBC51-C5B3-44DF-B2CF-B1EBF9347A2D}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DBD06261-84BB-4F0C-95FA-EC75EBC8F830}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0DDA82CE-4437-452F-A8C5-A05B74E969FC}">
           <x14:formula1>
             <xm:f>MethodsDropDown!$A$1:$A$103</xm:f>
           </x14:formula1>
@@ -2408,12 +2702,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF663E5-4D37-4BC8-9538-F213BED5A50A}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2436,31 +2730,31 @@
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
@@ -2486,10 +2780,10 @@
         <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>11</v>
+        <v>160</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>11</v>
@@ -2501,7 +2795,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -2513,7 +2807,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>11</v>
@@ -2534,10 +2828,10 @@
     </row>
     <row r="4" spans="1:11" ht="37.5">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
@@ -2546,7 +2840,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>11</v>
@@ -2567,7 +2861,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>16</v>
@@ -2633,7 +2927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C409FA-BE42-486D-A5BB-E789FEC45F4D}">
   <dimension ref="A1:K13"/>
   <sheetViews>
@@ -2661,31 +2955,31 @@
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
@@ -2693,10 +2987,10 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>11</v>
@@ -2726,10 +3020,10 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>11</v>
@@ -2759,10 +3053,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
@@ -2792,10 +3086,10 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>11</v>
@@ -2804,7 +3098,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>11</v>
@@ -2825,10 +3119,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>11</v>
@@ -2837,10 +3131,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>11</v>
@@ -2858,10 +3152,10 @@
     </row>
     <row r="7" spans="1:11" ht="25">
       <c r="A7" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>11</v>
@@ -2885,16 +3179,16 @@
         <v>11</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>11</v>
@@ -2924,11 +3218,11 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="C9" s="7" t="s">
         <v>11</v>
       </c>
@@ -2936,7 +3230,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>11</v>
@@ -2957,10 +3251,10 @@
     </row>
     <row r="10" spans="1:11" ht="25">
       <c r="A10" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>11</v>
@@ -2984,16 +3278,16 @@
         <v>11</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>11</v>
@@ -3023,10 +3317,10 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>11</v>
@@ -3056,10 +3350,10 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>11</v>
@@ -3122,461 +3416,415 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DC243D4-1802-4B2F-A8E1-29C13F5D35F7}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.90625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4" xr:uid="{31172039-31F4-40D8-A07C-07B2088B0032}">
+      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{B84BEFCF-B23D-47BD-9339-A47E1F0E0935}">
+      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{D8B78352-178C-4E82-B43C-257CA3FB785E}">
+      <formula1>"ios,android,cloudAndroid,cloudiOS,NA"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B7F41E-692A-4CA8-9ED3-CAEF988BE607}">
-  <dimension ref="A1:A88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF15D293-9E7B-4DB5-A90A-7077A9C8C42F}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="15.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.5">
+      <c r="A3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.5">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="3" t="s">
-        <v>154</v>
-      </c>
+      <c r="C4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>801742</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.5">
+      <c r="A5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="3"/>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{C74B8B57-87F6-4358-A16B-E2E274F68C56}">
+      <formula1>"ios,android,cloudAndroid,CloudiOS,NA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{CB583239-9D7D-4A1B-AE71-C48E4BC43385}">
+      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4" xr:uid="{345E68F6-2630-4998-85A7-A066C14B1EB0}">
+      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated flow which compatible with command line execution
</commit_message>
<xml_diff>
--- a/Testinput/Inputsheet.xlsx
+++ b/Testinput/Inputsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation-Workspace\Ymca\Testinput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0069B512-9105-48A2-9E78-3DCBCE99E10E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7691FC-3686-44E6-B2FF-BD9405821C4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="160">
   <si>
     <t>TCID</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>MOBILE PLATFORM</t>
-  </si>
-  <si>
-    <t>chrome</t>
   </si>
   <si>
     <t>TC003</t>
@@ -498,27 +495,9 @@
     <t>AndoidNextButton</t>
   </si>
   <si>
-    <t>android</t>
-  </si>
-  <si>
-    <t>ios</t>
-  </si>
-  <si>
-    <t>browserstack</t>
-  </si>
-  <si>
-    <t>browserstackchrome</t>
-  </si>
-  <si>
     <t>TC008</t>
   </si>
   <si>
-    <t>saucelabs</t>
-  </si>
-  <si>
-    <t>saucelabschrome</t>
-  </si>
-  <si>
     <t>AndroidTest</t>
   </si>
   <si>
@@ -532,9 +511,6 @@
   </si>
   <si>
     <t>SauceLabsTest</t>
-  </si>
-  <si>
-    <t>cloudAndroid</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1109,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1145,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
@@ -1154,10 +1130,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
@@ -1166,10 +1142,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -1178,10 +1154,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1190,10 +1166,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -1202,10 +1178,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
@@ -1214,10 +1190,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1262,7 +1238,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1287,407 +1263,407 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1697,10 +1673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD96CCB-A1A6-4ED0-8D30-67999F5EF9B1}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1711,15 +1687,12 @@
     <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.36328125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.90625" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="5"/>
+    <col min="7" max="7" width="18.54296875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1733,30 +1706,21 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:8">
       <c r="A2" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>10</v>
@@ -1773,29 +1737,20 @@
       <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="17" t="s">
-        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -1806,62 +1761,44 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="G3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="G4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -1872,42 +1809,22 @@
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="3"/>
+      <c r="G5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{46257E2C-578E-4299-893D-8DC7B6E23189}">
-      <formula1>"ios,android,cloudAndroid,CloudiOS,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{23951901-8F95-4C28-B671-572E3C0FB9DA}">
-      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4" xr:uid="{66E58A67-28A0-48BD-B382-68BF4E4214FB}">
-      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB22AF6-DB92-475E-8397-BFEB0405B8C4}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1918,15 +1835,12 @@
     <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.36328125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.90625" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="5"/>
+    <col min="7" max="7" width="18.54296875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1940,30 +1854,21 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:8">
       <c r="A2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>10</v>
@@ -1980,29 +1885,20 @@
       <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>14</v>
@@ -2013,29 +1909,20 @@
       <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="G3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>14</v>
@@ -2046,29 +1933,20 @@
       <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
@@ -2079,29 +1957,12 @@
       <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="3"/>
+      <c r="G5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{309AC59B-24DA-4A15-A9F3-AB3DB170B51F}">
-      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{4A666E9B-A5F6-4FD6-9CA1-75743DBF0E4C}">
-      <formula1>"ios,android,cloudAndroid,CloudiOS,NA"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2120,10 +1981,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E63851-4616-491C-89B9-1AFD437E032E}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -2133,15 +1994,12 @@
     <col min="3" max="3" width="13.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="5"/>
+    <col min="7" max="7" width="18.54296875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -2155,28 +2013,19 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -2196,20 +2045,11 @@
         <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11">
+        <v>11</v>
+      </c>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
@@ -2231,18 +2071,9 @@
       <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -2256,67 +2087,49 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>14</v>
@@ -2330,18 +2143,9 @@
       <c r="G6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -2363,30 +2167,12 @@
       <c r="G7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="11"/>
+      <c r="H7" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D2:D4" xr:uid="{389CF3E6-C2A5-41BF-92EC-6A12419D1103}">
       <formula1>"NA,xpath,id,name,linktext,partiallinktext"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{F80F15F2-9ED5-4625-8CC1-CA7C8E7A06CE}">
-      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{736DF6C9-394B-42D9-8F22-976925EEB67F}">
-      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{08A5DD28-C150-413D-B303-3AA6BCA0C992}">
-      <formula1>"ios,android,NA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -2412,10 +2198,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFA2299-BAF5-4AEB-8201-9BE12BC72674}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -2425,15 +2211,12 @@
     <col min="3" max="3" width="13.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="5"/>
+    <col min="7" max="7" width="18.54296875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -2447,28 +2230,19 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -2488,20 +2262,11 @@
         <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11">
+        <v>11</v>
+      </c>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
@@ -2523,18 +2288,9 @@
       <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -2548,67 +2304,49 @@
         <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>14</v>
@@ -2622,18 +2360,9 @@
       <c r="G6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -2655,28 +2384,10 @@
       <c r="G7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="11"/>
+      <c r="H7" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{25F55D36-9777-4009-A415-EC6180727EA8}">
-      <formula1>"ios,android,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{BB2605B6-0E53-4E54-BE61-FD1BB39326EF}">
-      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{307608A3-E9A9-4B8B-BBE5-81D2DE6262A1}">
-      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D2:D4" xr:uid="{F9AF23F6-16A3-4F2C-8DDE-2BD1876D8B36}">
       <formula1>"NA,xpath,id,name,linktext,partiallinktext"</formula1>
     </dataValidation>
@@ -2704,10 +2415,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF663E5-4D37-4BC8-9538-F213BED5A50A}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2718,14 +2429,11 @@
     <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.90625" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="5"/>
+    <col min="7" max="7" width="18.54296875" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -2739,28 +2447,19 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -2780,20 +2479,11 @@
         <v>11</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11">
+        <v>11</v>
+      </c>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>25</v>
       </c>
@@ -2807,7 +2497,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>11</v>
@@ -2815,18 +2505,9 @@
       <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" ht="37.5">
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" ht="37.5">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -2840,7 +2521,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>11</v>
@@ -2848,18 +2529,9 @@
       <c r="G4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -2881,30 +2553,12 @@
       <c r="G5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="11"/>
+      <c r="H5" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{BCAA54BC-B7D0-40F7-9463-BC5249218B09}">
       <formula1>"NA,xpath,id,name,linktext,partiallinktext"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{A07DF584-5344-4508-BD8F-A58A06C5C6B8}">
-      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{7855E6D5-7CC0-49B5-A47B-725CA7523040}">
-      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{F4B9FC72-F97E-4CD9-9D32-CE1A1E1A57C6}">
-      <formula1>"ios,android,NA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -2929,10 +2583,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C409FA-BE42-486D-A5BB-E789FEC45F4D}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2943,14 +2597,11 @@
     <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="5"/>
+    <col min="7" max="7" width="18.54296875" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -2964,67 +2615,49 @@
         <v>18</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
@@ -3040,254 +2673,182 @@
       <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="25">
+      <c r="A7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="B8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="25">
-      <c r="A7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="12" t="s">
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="25">
+      <c r="A10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" ht="25">
-      <c r="A10" s="7" t="s">
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>11</v>
@@ -3301,26 +2862,17 @@
       <c r="F11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="G11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>11</v>
@@ -3334,26 +2886,17 @@
       <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="G12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>11</v>
@@ -3367,36 +2910,15 @@
       <c r="F13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="9"/>
+      <c r="G13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="9"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I13" xr:uid="{D75DDDFB-D638-4F2F-9757-08FDD4CC8696}">
-      <formula1>"ios,android,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G13" xr:uid="{2B969699-C2F1-4E45-9156-30B62C4EDC92}">
-      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H13" xr:uid="{349CF3F5-6150-4946-B998-3FD1456ADD9B}">
-      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13" xr:uid="{FE594086-A6A1-4D54-B1B5-F282E6D45761}">
       <formula1>"NA,xpath,id,name,linktext,partiallinktext"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{8DD37748-9824-43A5-ABC8-AF2CADB5B9FF}">
-      <formula1>"ios,android,cloudAndroid,CloudiOS,NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3418,10 +2940,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DC243D4-1802-4B2F-A8E1-29C13F5D35F7}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -3431,15 +2953,12 @@
     <col min="3" max="3" width="15" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.90625" style="5"/>
+    <col min="7" max="7" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.90625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -3453,30 +2972,21 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:8">
       <c r="A2" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>10</v>
@@ -3493,29 +3003,20 @@
       <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="17" t="s">
-        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -3526,62 +3027,44 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="G3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="G4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -3592,32 +3075,12 @@
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="3"/>
+      <c r="G5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 G4" xr:uid="{31172039-31F4-40D8-A07C-07B2088B0032}">
-      <formula1>"chrome,firefox,ie,browserstackchrome,browserstackfirefox,browserstackie,saucelabschrome,saucelabsfirefox,saucelabsie,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{B84BEFCF-B23D-47BD-9339-A47E1F0E0935}">
-      <formula1>"browserstack,saucelabs,mobile,NA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{D8B78352-178C-4E82-B43C-257CA3FB785E}">
-      <formula1>"ios,android,cloudAndroid,cloudiOS,NA"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3660,10 +3123,10 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>26</v>
@@ -3675,7 +3138,7 @@
         <v>28</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>8</v>
@@ -3683,7 +3146,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>10</v>
@@ -3704,10 +3167,10 @@
         <v>11</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>11</v>
@@ -3716,13 +3179,13 @@
     </row>
     <row r="3" spans="1:11" ht="15.5">
       <c r="A3" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>14</v>
@@ -3749,13 +3212,13 @@
     </row>
     <row r="4" spans="1:11" ht="15.5">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>14</v>
@@ -3782,13 +3245,13 @@
     </row>
     <row r="5" spans="1:11" ht="15.5">
       <c r="A5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>14</v>

</xml_diff>